<commit_message>
using priority queue, improved performance
</commit_message>
<xml_diff>
--- a/Energy Consumption0.xlsx
+++ b/Energy Consumption0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.644626596487287</v>
+        <v>2.613752437523362</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6049290408927925</v>
+        <v>0.7592657640396985</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3.169238891737946</v>
+        <v>2.716536614101855</v>
       </c>
       <c r="C3" t="n">
-        <v>1.605332351139208</v>
+        <v>1.460595639285859</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3.276602654645827</v>
+        <v>7.041282202434871</v>
       </c>
       <c r="C4" t="n">
-        <v>2.279382393567999</v>
+        <v>2.304059489169519</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>10.5344789910152</v>
+        <v>12.03599109472344</v>
       </c>
       <c r="C5" t="n">
-        <v>3.433665371404484</v>
+        <v>3.173738742024204</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>10.60055246648265</v>
+        <v>14.6921863375777</v>
       </c>
       <c r="C6" t="n">
-        <v>4.01749298408938</v>
+        <v>4.001888878368169</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11.2756946898995</v>
+        <v>21.57270026272947</v>
       </c>
       <c r="C7" t="n">
-        <v>4.997671327413242</v>
+        <v>4.887993696444225</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>13.63479151027687</v>
+        <v>21.68642128141905</v>
       </c>
       <c r="C8" t="n">
-        <v>5.528976015675983</v>
+        <v>5.959203634897216</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>13.75165502487991</v>
+        <v>22.12642842980381</v>
       </c>
       <c r="C9" t="n">
-        <v>6.152833773684079</v>
+        <v>6.876654006919253</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>13.85075693868946</v>
+        <v>22.43733789614787</v>
       </c>
       <c r="C10" t="n">
-        <v>6.835485082155865</v>
+        <v>7.845604822855141</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19.16286694082578</v>
+        <v>22.47942909118693</v>
       </c>
       <c r="C11" t="n">
-        <v>7.666510727511255</v>
+        <v>8.645824804633929</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19.25096971237213</v>
+        <v>23.68583780630273</v>
       </c>
       <c r="C12" t="n">
-        <v>8.281634792542798</v>
+        <v>9.651851359695083</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19.94387999121192</v>
+        <v>24.6012085290772</v>
       </c>
       <c r="C13" t="n">
-        <v>8.911532212119297</v>
+        <v>10.37624620878069</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20.63812998014084</v>
+        <v>26.95666560595685</v>
       </c>
       <c r="C14" t="n">
-        <v>9.727553789424393</v>
+        <v>11.0979363918407</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>23.00933880177545</v>
+        <v>28.51084660616283</v>
       </c>
       <c r="C15" t="n">
-        <v>10.32656284248386</v>
+        <v>11.94586713835366</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>23.12533110181544</v>
+        <v>28.64542511507138</v>
       </c>
       <c r="C16" t="n">
-        <v>11.07871474078948</v>
+        <v>12.88993087357854</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>23.81676410386505</v>
+        <v>30.00697626199472</v>
       </c>
       <c r="C17" t="n">
-        <v>11.95198329443012</v>
+        <v>13.73978214927143</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>23.85730590642074</v>
+        <v>30.18160745226803</v>
       </c>
       <c r="C18" t="n">
-        <v>12.40655709478213</v>
+        <v>14.9431245371633</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>23.95085213732904</v>
+        <v>32.29221835264032</v>
       </c>
       <c r="C19" t="n">
-        <v>13.03854019197044</v>
+        <v>15.84098931660236</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>27.50533553788397</v>
+        <v>36.68977613810812</v>
       </c>
       <c r="C20" t="n">
-        <v>14.00033151391241</v>
+        <v>16.71748676836768</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>27.67661460221781</v>
+        <v>39.24058746232968</v>
       </c>
       <c r="C21" t="n">
-        <v>14.60159111544923</v>
+        <v>17.65458176062602</v>
       </c>
     </row>
     <row r="22">
@@ -670,10 +670,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>31.20706613690617</v>
+        <v>42.45769340898283</v>
       </c>
       <c r="C22" t="n">
-        <v>15.24286729106726</v>
+        <v>18.38999985699175</v>
       </c>
     </row>
     <row r="23">
@@ -681,10 +681,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>37.26365396804432</v>
+        <v>42.72038277164717</v>
       </c>
       <c r="C23" t="n">
-        <v>15.99801577580338</v>
+        <v>19.29597632478046</v>
       </c>
     </row>
     <row r="24">
@@ -692,10 +692,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>37.61697401534485</v>
+        <v>47.12024772749498</v>
       </c>
       <c r="C24" t="n">
-        <v>16.56107973117251</v>
+        <v>20.06302809841178</v>
       </c>
     </row>
     <row r="25">
@@ -703,10 +703,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>47.45983733097311</v>
+        <v>47.18983974099818</v>
       </c>
       <c r="C25" t="n">
-        <v>17.26825230347642</v>
+        <v>20.84046645116023</v>
       </c>
     </row>
     <row r="26">
@@ -714,10 +714,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>47.59064220376185</v>
+        <v>47.45139448397205</v>
       </c>
       <c r="C26" t="n">
-        <v>18.06915891925957</v>
+        <v>21.73050188173235</v>
       </c>
     </row>
     <row r="27">
@@ -725,10 +725,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>53.69933808013098</v>
+        <v>57.08002863459992</v>
       </c>
       <c r="C27" t="n">
-        <v>19.41425070668806</v>
+        <v>22.53922142054101</v>
       </c>
     </row>
     <row r="28">
@@ -736,10 +736,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>53.84585199676497</v>
+        <v>57.19176874318924</v>
       </c>
       <c r="C28" t="n">
-        <v>19.94615839508295</v>
+        <v>23.46843318447786</v>
       </c>
     </row>
     <row r="29">
@@ -747,10 +747,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>56.70013704534426</v>
+        <v>57.75826233793363</v>
       </c>
       <c r="C29" t="n">
-        <v>20.51382085820509</v>
+        <v>24.32965619625855</v>
       </c>
     </row>
     <row r="30">
@@ -758,10 +758,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>56.9071178756293</v>
+        <v>59.94346593310251</v>
       </c>
       <c r="C30" t="n">
-        <v>21.3356761432659</v>
+        <v>25.51196157872716</v>
       </c>
     </row>
     <row r="31">
@@ -769,10 +769,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>59.59098436640628</v>
+        <v>62.82205560266711</v>
       </c>
       <c r="C31" t="n">
-        <v>21.93548470518899</v>
+        <v>26.38783686786138</v>
       </c>
     </row>
     <row r="32">
@@ -780,10 +780,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>59.64226324053019</v>
+        <v>62.8817530065571</v>
       </c>
       <c r="C32" t="n">
-        <v>22.78440071629584</v>
+        <v>27.30969612916372</v>
       </c>
     </row>
     <row r="33">
@@ -791,10 +791,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>70.82576908155666</v>
+        <v>72.54148468743868</v>
       </c>
       <c r="C33" t="n">
-        <v>23.62003760965211</v>
+        <v>28.040704622941</v>
       </c>
     </row>
     <row r="34">
@@ -802,10 +802,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>72.17566288790181</v>
+        <v>72.97501644923719</v>
       </c>
       <c r="C34" t="n">
-        <v>24.15283060978762</v>
+        <v>28.84470881218256</v>
       </c>
     </row>
     <row r="35">
@@ -813,10 +813,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>76.39257863190426</v>
+        <v>73.06838145081315</v>
       </c>
       <c r="C35" t="n">
-        <v>24.71521484977792</v>
+        <v>29.75031308741781</v>
       </c>
     </row>
     <row r="36">
@@ -824,10 +824,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>81.9266316003644</v>
+        <v>75.27802637213172</v>
       </c>
       <c r="C36" t="n">
-        <v>25.30224752763654</v>
+        <v>30.48428657400807</v>
       </c>
     </row>
     <row r="37">
@@ -835,10 +835,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>82.0297006384543</v>
+        <v>78.20291173745026</v>
       </c>
       <c r="C37" t="n">
-        <v>26.05903817678816</v>
+        <v>31.46848739832284</v>
       </c>
     </row>
     <row r="38">
@@ -846,10 +846,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>83.0566942469022</v>
+        <v>78.29546518141368</v>
       </c>
       <c r="C38" t="n">
-        <v>26.88404040871227</v>
+        <v>32.30596951609363</v>
       </c>
     </row>
     <row r="39">
@@ -857,10 +857,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>83.18535866819147</v>
+        <v>78.60360553774709</v>
       </c>
       <c r="C39" t="n">
-        <v>27.61422509159538</v>
+        <v>33.14985736365251</v>
       </c>
     </row>
     <row r="40">
@@ -868,10 +868,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>83.3211684899892</v>
+        <v>79.72355933701955</v>
       </c>
       <c r="C40" t="n">
-        <v>28.41787507735054</v>
+        <v>33.99770763239682</v>
       </c>
     </row>
     <row r="41">
@@ -879,10 +879,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>83.80402033155104</v>
+        <v>79.80473470598035</v>
       </c>
       <c r="C41" t="n">
-        <v>29.00032312125697</v>
+        <v>34.88410236901647</v>
       </c>
     </row>
     <row r="42">
@@ -890,10 +890,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>83.98141493475619</v>
+        <v>94.34852273764618</v>
       </c>
       <c r="C42" t="n">
-        <v>29.60796551255223</v>
+        <v>35.82076498679206</v>
       </c>
     </row>
     <row r="43">
@@ -901,10 +901,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>84.04645017828324</v>
+        <v>94.47171610910208</v>
       </c>
       <c r="C43" t="n">
-        <v>30.14924233767338</v>
+        <v>36.7427201892187</v>
       </c>
     </row>
     <row r="44">
@@ -912,10 +912,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>86.44017175025351</v>
+        <v>94.58400135795851</v>
       </c>
       <c r="C44" t="n">
-        <v>30.722673815642</v>
+        <v>37.50748567541343</v>
       </c>
     </row>
     <row r="45">
@@ -923,10 +923,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>86.57779960787425</v>
+        <v>95.01755374451145</v>
       </c>
       <c r="C45" t="n">
-        <v>31.27470440733439</v>
+        <v>38.35212812944956</v>
       </c>
     </row>
     <row r="46">
@@ -934,10 +934,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>86.76617184783262</v>
+        <v>98.58123591599718</v>
       </c>
       <c r="C46" t="n">
-        <v>32.11947600796123</v>
+        <v>39.21071623763321</v>
       </c>
     </row>
     <row r="47">
@@ -945,10 +945,21 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>91.93741823959488</v>
+        <v>98.99359252344701</v>
       </c>
       <c r="C47" t="n">
-        <v>32.98555963472404</v>
+        <v>40.56455204753814</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>99.23171059013568</v>
+      </c>
+      <c r="C48" t="n">
+        <v>41.37185266170029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>